<commit_message>
Interfaz de partida y reportes implementados
</commit_message>
<xml_diff>
--- a/assets/info/plantilla-reportes-reforma.xlsx
+++ b/assets/info/plantilla-reportes-reforma.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">REPORTE REFORMA JUDICIAL</t>
   </si>
@@ -28,7 +28,19 @@
     <t xml:space="preserve">No</t>
   </si>
   <si>
+    <t xml:space="preserve">NOMBRES</t>
+  </si>
+  <si>
     <t xml:space="preserve">CI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FECHA NACIMIENTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No LIBRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No PARTIDA</t>
   </si>
   <si>
     <t xml:space="preserve">USUARIO</t>
@@ -319,9 +331,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>982080</xdr:colOff>
+      <xdr:colOff>981720</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>45360</xdr:rowOff>
+      <xdr:rowOff>45000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -335,7 +347,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="314280"/>
-          <a:ext cx="3585600" cy="1121400"/>
+          <a:ext cx="3585240" cy="1121040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -357,8 +369,8 @@
   </sheetPr>
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -421,10 +433,18 @@
       <c r="C5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="11"/>
+      <c r="D5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>

</xml_diff>

<commit_message>
Validadores modificados, campo AE agregado
</commit_message>
<xml_diff>
--- a/assets/info/plantilla-reportes-reforma.xlsx
+++ b/assets/info/plantilla-reportes-reforma.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">REPORTE REFORMA JUDICIAL</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t xml:space="preserve">NOMBRES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APELLIDO ESPOSO</t>
   </si>
   <si>
     <t xml:space="preserve">CI</t>
@@ -327,13 +330,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>66600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:rowOff>29160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>981720</xdr:colOff>
+      <xdr:colOff>981360</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>45000</xdr:rowOff>
+      <xdr:rowOff>44640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -346,8 +349,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="66600" y="314280"/>
-          <a:ext cx="3585240" cy="1121040"/>
+          <a:off x="66600" y="308880"/>
+          <a:ext cx="3584880" cy="1120680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -367,33 +370,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="46.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="59.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="39.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="26.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="29.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="34.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="43.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="4" width="40.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="37.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="4" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="28.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="46.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="59.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="39.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="26.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="29.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="34.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="4" width="43.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="40.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="4" width="37.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="4" width="11.42"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -406,22 +409,23 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" s="4" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" s="4" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="6"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" s="4" customFormat="true" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
@@ -433,7 +437,7 @@
       <c r="C5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="12" t="s">
@@ -442,10 +446,12 @@
       <c r="F5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="11"/>
+      <c r="H5" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
@@ -453,22 +459,23 @@
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="G6:G1048576 G1">
+  <conditionalFormatting sqref="H6:H1048576 H1">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Reforma Electoral" dxfId="0">
-      <formula>NOT(ISERROR(SEARCH("Reforma Electoral",G1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Reforma Electoral",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
+  <conditionalFormatting sqref="H1:H1048576">
     <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Censo" dxfId="1">
-      <formula>NOT(ISERROR(SEARCH("Censo",G1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Censo",H1)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Institucionalidad Democratica" dxfId="2">
-      <formula>NOT(ISERROR(SEARCH("Institucionalidad Democratica",G1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Institucionalidad Democratica",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>